<commit_message>
Script to seed players and player_stats database tables with data from the players spreadsheet.
</commit_message>
<xml_diff>
--- a/fifa_player_recommendation_system/data/teams.xlsx
+++ b/fifa_player_recommendation_system/data/teams.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Projects\FIFA-Player-Recommendation-System\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Projects\FIFA-Player-Recommendation-System\fifa_player_recommendation_system\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556FA4C6-A59B-4743-80ED-82D548BEEF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F2850B-0D35-4265-A05E-53CA513512BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9B5FE3FD-CC0C-4DC9-877F-8A6B1F848B45}"/>
   </bookViews>
@@ -1412,9 +1412,6 @@
     <t>Ternana</t>
   </si>
   <si>
-    <t xml:space="preserve">Urbs Reggina 1914 </t>
-  </si>
-  <si>
     <t>Venezia FC</t>
   </si>
   <si>
@@ -1622,9 +1619,6 @@
     <t>Warta Poznań</t>
   </si>
   <si>
-    <t>Widzew Åódź</t>
-  </si>
-  <si>
     <t>Wisła Płock</t>
   </si>
   <si>
@@ -1724,9 +1718,6 @@
     <t>UCD AFC</t>
   </si>
   <si>
-    <t>AFC Chindia Târgoviște</t>
-  </si>
-  <si>
     <t>Romanian Liga I</t>
   </si>
   <si>
@@ -1745,9 +1736,6 @@
     <t>Campionii FC Arges</t>
   </si>
   <si>
-    <t>FC Botoșani</t>
-  </si>
-  <si>
     <t>FC Farul Constanța</t>
   </si>
   <si>
@@ -1760,12 +1748,6 @@
     <t>FCSB (Steaua)</t>
   </si>
   <si>
-    <t>Petrolul Ploiești</t>
-  </si>
-  <si>
-    <t>Rapid București</t>
-  </si>
-  <si>
     <t>Sepsi OSK Sf. Gheorghe</t>
   </si>
   <si>
@@ -2039,15 +2021,9 @@
     <t>Antalyaspor</t>
   </si>
   <si>
-    <t>Atakaș Hatayspor</t>
-  </si>
-  <si>
     <t>Aytemiz Alanyaspor</t>
   </si>
   <si>
-    <t>Beșiktaș JK</t>
-  </si>
-  <si>
     <t>Demir Grup Sivasspor</t>
   </si>
   <si>
@@ -2063,12 +2039,6 @@
     <t>Galatasaray SK</t>
   </si>
   <si>
-    <t>Gazișehir Gaziantep F.K.</t>
-  </si>
-  <si>
-    <t>Kasimpașa SK</t>
-  </si>
-  <si>
     <t>MKE Ankaragücü</t>
   </si>
   <si>
@@ -2081,9 +2051,6 @@
     <t>Ümraniyespor</t>
   </si>
   <si>
-    <t>İstanbul Bașakșehir FK</t>
-  </si>
-  <si>
     <t>İstanbulspor</t>
   </si>
   <si>
@@ -2232,6 +2199,39 @@
   </si>
   <si>
     <t>Metropolitanos de Caracas FC</t>
+  </si>
+  <si>
+    <t>Beşiktaş JK</t>
+  </si>
+  <si>
+    <t>İstanbul Başakşehir FK</t>
+  </si>
+  <si>
+    <t>Gazişehir Gaziantep F.K.</t>
+  </si>
+  <si>
+    <t>Atakaş Hatayspor</t>
+  </si>
+  <si>
+    <t>Kasimpaşa SK</t>
+  </si>
+  <si>
+    <t>Urbs Reggina 1914</t>
+  </si>
+  <si>
+    <t>Petrolul Ploieşti</t>
+  </si>
+  <si>
+    <t>Rapid Bucureşti</t>
+  </si>
+  <si>
+    <t>FC Botoşani</t>
+  </si>
+  <si>
+    <t>Widzew Łódź</t>
+  </si>
+  <si>
+    <t>AFC Chindia Târgovişte</t>
   </si>
 </sst>
 </file>
@@ -2584,7 +2584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2594,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC94B1D8-6C12-435F-93A9-A6DE54618C0E}">
   <dimension ref="A1:B679"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A502" workbookViewId="0">
+      <selection activeCell="B523" sqref="B523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6014,7 +6014,7 @@
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>458</v>
+        <v>726</v>
       </c>
       <c r="B427" t="s">
         <v>440</v>
@@ -6022,7 +6022,7 @@
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B428" t="s">
         <v>440</v>
@@ -6030,2010 +6030,2010 @@
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
+        <v>459</v>
+      </c>
+      <c r="B429" t="s">
         <v>460</v>
-      </c>
-      <c r="B429" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B430" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B431" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B432" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B433" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B434" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B435" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B436" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B437" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B438" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B439" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B440" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
+        <v>472</v>
+      </c>
+      <c r="B441" t="s">
         <v>473</v>
-      </c>
-      <c r="B441" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B442" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B443" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B444" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B445" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B446" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B447" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
+        <v>480</v>
+      </c>
+      <c r="B448" t="s">
         <v>481</v>
-      </c>
-      <c r="B448" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B449" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B450" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B451" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B452" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B453" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B454" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B455" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B456" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B457" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B458" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B459" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B460" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B461" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B462" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B463" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
+        <v>497</v>
+      </c>
+      <c r="B464" t="s">
         <v>498</v>
-      </c>
-      <c r="B464" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B465" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B466" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B467" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B468" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B469" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B470" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
+        <v>505</v>
+      </c>
+      <c r="B471" t="s">
         <v>506</v>
-      </c>
-      <c r="B471" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B472" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B473" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B474" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B475" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B476" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
+        <v>512</v>
+      </c>
+      <c r="B477" t="s">
         <v>513</v>
-      </c>
-      <c r="B477" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B478" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B479" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B480" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B481" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B482" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B483" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B484" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B485" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B486" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B487" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B488" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B489" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B490" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>528</v>
+        <v>730</v>
       </c>
       <c r="B491" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B492" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B493" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B494" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B495" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B496" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B497" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B498" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B499" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B500" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B501" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B502" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B503" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B504" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B505" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B506" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B507" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B508" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B509" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B510" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B511" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B512" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B513" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B514" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B515" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B516" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B517" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B518" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B519" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B520" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B521" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B522" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>562</v>
+        <v>731</v>
       </c>
       <c r="B523" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B524" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B525" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B526" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B527" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B528" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>569</v>
+        <v>729</v>
       </c>
       <c r="B529" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B530" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B531" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B532" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B533" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>574</v>
+        <v>727</v>
       </c>
       <c r="B534" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>575</v>
+        <v>728</v>
       </c>
       <c r="B535" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B536" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="B537" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="B538" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="B539" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="B540" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="B541" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B542" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="B543" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B544" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="B545" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="B546" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B547" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="B548" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="B549" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="B550" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="B551" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="B552" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="B553" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="B554" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B555" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="B556" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="B557" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="B558" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="B559" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="B560" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B561" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="B562" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="B563" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="B564" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B565" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="B566" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="B567" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B568" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="B569" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B570" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="B571" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B572" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="B573" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="B574" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="B575" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="B576" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B577" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="B578" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B579" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B580" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="B581" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="B582" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="B583" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="B584" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B585" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="B586" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="B587" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="B588" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="B589" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="B590" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="B591" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="B592" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="B593" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="B594" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="B595" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="B596" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B597" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="B598" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="B599" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="B600" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="B601" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="B602" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="B603" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="B604" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="B605" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="B606" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="B607" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="B608" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="B609" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="B610" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="B611" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="B612" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B613" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B614" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="B615" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="B616" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="B617" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="B618" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="B619" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>667</v>
+        <v>724</v>
       </c>
       <c r="B620" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="B621" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>669</v>
+        <v>721</v>
       </c>
       <c r="B622" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B623" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="B624" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="B625" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="B626" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="B627" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>675</v>
+        <v>723</v>
       </c>
       <c r="B628" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>676</v>
+        <v>725</v>
       </c>
       <c r="B629" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="B630" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>678</v>
+        <v>668</v>
       </c>
       <c r="B631" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>679</v>
+        <v>669</v>
       </c>
       <c r="B632" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="B633" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="B634" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>682</v>
+        <v>671</v>
       </c>
       <c r="B635" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>683</v>
+        <v>672</v>
       </c>
       <c r="B636" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>684</v>
+        <v>673</v>
       </c>
       <c r="B637" t="s">
-        <v>685</v>
+        <v>674</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>686</v>
+        <v>675</v>
       </c>
       <c r="B638" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>688</v>
+        <v>677</v>
       </c>
       <c r="B639" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
       <c r="B640" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>690</v>
+        <v>679</v>
       </c>
       <c r="B641" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>691</v>
+        <v>680</v>
       </c>
       <c r="B642" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>692</v>
+        <v>681</v>
       </c>
       <c r="B643" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>693</v>
+        <v>682</v>
       </c>
       <c r="B644" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>694</v>
+        <v>683</v>
       </c>
       <c r="B645" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>695</v>
+        <v>684</v>
       </c>
       <c r="B646" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>696</v>
+        <v>685</v>
       </c>
       <c r="B647" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>697</v>
+        <v>686</v>
       </c>
       <c r="B648" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>698</v>
+        <v>687</v>
       </c>
       <c r="B649" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
       <c r="B650" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>700</v>
+        <v>689</v>
       </c>
       <c r="B651" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>701</v>
+        <v>690</v>
       </c>
       <c r="B652" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>702</v>
+        <v>691</v>
       </c>
       <c r="B653" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>703</v>
+        <v>692</v>
       </c>
       <c r="B654" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>704</v>
+        <v>693</v>
       </c>
       <c r="B655" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>705</v>
+        <v>694</v>
       </c>
       <c r="B656" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="B657" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
       <c r="B658" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>708</v>
+        <v>697</v>
       </c>
       <c r="B659" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>709</v>
+        <v>698</v>
       </c>
       <c r="B660" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>710</v>
+        <v>699</v>
       </c>
       <c r="B661" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>711</v>
+        <v>700</v>
       </c>
       <c r="B662" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>712</v>
+        <v>701</v>
       </c>
       <c r="B663" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>713</v>
+        <v>702</v>
       </c>
       <c r="B664" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>714</v>
+        <v>703</v>
       </c>
       <c r="B665" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>715</v>
+        <v>704</v>
       </c>
       <c r="B666" t="s">
-        <v>716</v>
+        <v>705</v>
       </c>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>717</v>
+        <v>706</v>
       </c>
       <c r="B667" t="s">
-        <v>716</v>
+        <v>705</v>
       </c>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="B668" t="s">
-        <v>719</v>
+        <v>708</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>720</v>
+        <v>709</v>
       </c>
       <c r="B669" t="s">
-        <v>719</v>
+        <v>708</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>721</v>
+        <v>710</v>
       </c>
       <c r="B670" t="s">
-        <v>719</v>
+        <v>708</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>722</v>
+        <v>711</v>
       </c>
       <c r="B671" t="s">
-        <v>719</v>
+        <v>708</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>723</v>
+        <v>712</v>
       </c>
       <c r="B672" t="s">
-        <v>719</v>
+        <v>708</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>724</v>
+        <v>713</v>
       </c>
       <c r="B673" t="s">
-        <v>719</v>
+        <v>708</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>725</v>
+        <v>714</v>
       </c>
       <c r="B674" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>727</v>
+        <v>716</v>
       </c>
       <c r="B675" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>728</v>
+        <v>717</v>
       </c>
       <c r="B676" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>729</v>
+        <v>718</v>
       </c>
       <c r="B677" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>730</v>
+        <v>719</v>
       </c>
       <c r="B678" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>731</v>
+        <v>720</v>
       </c>
       <c r="B679" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>